<commit_message>
Update dữ liệu chỉnh sửa
</commit_message>
<xml_diff>
--- a/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Cap nhat dia diem/CF0142_BAChecklistERP.xlsx
+++ b/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Cap nhat dia diem/CF0142_BAChecklistERP.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SOFT\201512\10_DOCUMENT\13_DETAIL_DESIGN\Cap nhat dia diem\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" tabRatio="653" activeTab="2"/>
   </bookViews>
@@ -15,12 +20,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Layout!$A$1:$K$44</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="127">
   <si>
     <t>STT</t>
   </si>
@@ -415,7 +420,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -713,26 +718,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -776,6 +763,27 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -805,9 +813,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1150,7 +1155,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1182,9 +1187,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1216,6 +1222,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1391,7 +1398,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W44"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="93" zoomScaleSheetLayoutView="93" workbookViewId="0">
@@ -1426,16 +1433,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="37" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
       <c r="J1" s="2" t="s">
         <v>25</v>
       </c>
@@ -1444,28 +1451,28 @@
       </c>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
       <c r="J2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="15.75">
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
       <c r="J3" s="2" t="s">
         <v>27</v>
       </c>
@@ -1507,94 +1514,94 @@
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:23">
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="43" t="s">
+      <c r="F7" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="34" t="s">
+      <c r="G7" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="34"/>
-      <c r="I7" s="28" t="s">
+      <c r="H7" s="49"/>
+      <c r="I7" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="29"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="28" t="s">
+      <c r="J7" s="44"/>
+      <c r="K7" s="45"/>
+      <c r="L7" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="29"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="28" t="s">
+      <c r="M7" s="44"/>
+      <c r="N7" s="45"/>
+      <c r="O7" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="28" t="s">
+      <c r="P7" s="44"/>
+      <c r="Q7" s="45"/>
+      <c r="R7" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="S7" s="29"/>
-      <c r="T7" s="30"/>
-      <c r="U7" s="28" t="s">
+      <c r="S7" s="44"/>
+      <c r="T7" s="45"/>
+      <c r="U7" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="V7" s="29"/>
-      <c r="W7" s="30"/>
+      <c r="V7" s="44"/>
+      <c r="W7" s="45"/>
     </row>
     <row r="8" spans="1:23">
-      <c r="B8" s="44"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="31" t="s">
+      <c r="B8" s="38"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="H8" s="33"/>
-      <c r="I8" s="31" t="s">
+      <c r="H8" s="48"/>
+      <c r="I8" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="J8" s="32"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="31" t="s">
+      <c r="J8" s="47"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="32"/>
-      <c r="N8" s="33"/>
-      <c r="O8" s="31" t="s">
+      <c r="M8" s="47"/>
+      <c r="N8" s="48"/>
+      <c r="O8" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="P8" s="32"/>
-      <c r="Q8" s="33"/>
-      <c r="R8" s="31" t="s">
+      <c r="P8" s="47"/>
+      <c r="Q8" s="48"/>
+      <c r="R8" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="S8" s="32"/>
-      <c r="T8" s="33"/>
-      <c r="U8" s="31" t="s">
+      <c r="S8" s="47"/>
+      <c r="T8" s="48"/>
+      <c r="U8" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="V8" s="32"/>
-      <c r="W8" s="33"/>
+      <c r="V8" s="47"/>
+      <c r="W8" s="48"/>
     </row>
     <row r="9" spans="1:23" ht="28.5">
       <c r="A9" s="6"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="7" t="s">
         <v>17</v>
       </c>
@@ -1654,7 +1661,7 @@
       <c r="C10" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="29" t="s">
         <v>34</v>
       </c>
       <c r="E10" s="18" t="s">
@@ -1690,7 +1697,7 @@
       <c r="C11" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D11" s="35"/>
+      <c r="D11" s="29"/>
       <c r="E11" s="19" t="s">
         <v>36</v>
       </c>
@@ -1724,7 +1731,7 @@
       <c r="C12" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="35"/>
+      <c r="D12" s="29"/>
       <c r="E12" s="19" t="s">
         <v>37</v>
       </c>
@@ -1758,7 +1765,7 @@
       <c r="C13" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="35"/>
+      <c r="D13" s="29"/>
       <c r="E13" s="18" t="s">
         <v>39</v>
       </c>
@@ -1792,7 +1799,7 @@
       <c r="C14" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="35"/>
+      <c r="D14" s="29"/>
       <c r="E14" s="18" t="s">
         <v>35</v>
       </c>
@@ -1824,7 +1831,7 @@
       <c r="C15" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D15" s="35"/>
+      <c r="D15" s="29"/>
       <c r="E15" s="20" t="s">
         <v>63</v>
       </c>
@@ -2675,14 +2682,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="D10:D15"/>
-    <mergeCell ref="B1:D3"/>
-    <mergeCell ref="E1:I3"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="C7:C9"/>
     <mergeCell ref="U7:W7"/>
     <mergeCell ref="U8:W8"/>
     <mergeCell ref="O7:Q7"/>
@@ -2695,6 +2694,14 @@
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="L8:N8"/>
+    <mergeCell ref="D10:D15"/>
+    <mergeCell ref="B1:D3"/>
+    <mergeCell ref="E1:I3"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="C7:C9"/>
   </mergeCells>
   <conditionalFormatting sqref="G10:G40 I10:J40 L10:M40 O10:P40 R10:S40 U10:V40">
     <cfRule type="expression" dxfId="13" priority="15">
@@ -2728,11 +2735,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W43"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="C13" zoomScaleNormal="55" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView view="pageBreakPreview" topLeftCell="F16" zoomScaleNormal="55" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2759,16 +2766,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="37" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
       <c r="J1" s="2" t="s">
         <v>25</v>
       </c>
@@ -2777,28 +2784,28 @@
       </c>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
       <c r="J2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
       <c r="J3" s="2" t="s">
         <v>27</v>
       </c>
@@ -2838,94 +2845,94 @@
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:23">
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="43" t="s">
+      <c r="F7" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="34" t="s">
+      <c r="G7" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="34"/>
-      <c r="I7" s="28" t="s">
+      <c r="H7" s="49"/>
+      <c r="I7" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="29"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="28" t="s">
+      <c r="J7" s="44"/>
+      <c r="K7" s="45"/>
+      <c r="L7" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="29"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="28" t="s">
+      <c r="M7" s="44"/>
+      <c r="N7" s="45"/>
+      <c r="O7" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="28" t="s">
+      <c r="P7" s="44"/>
+      <c r="Q7" s="45"/>
+      <c r="R7" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="S7" s="29"/>
-      <c r="T7" s="30"/>
-      <c r="U7" s="28" t="s">
+      <c r="S7" s="44"/>
+      <c r="T7" s="45"/>
+      <c r="U7" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="V7" s="29"/>
-      <c r="W7" s="30"/>
+      <c r="V7" s="44"/>
+      <c r="W7" s="45"/>
     </row>
     <row r="8" spans="1:23">
-      <c r="B8" s="44"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="31" t="s">
+      <c r="B8" s="38"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="H8" s="33"/>
-      <c r="I8" s="31" t="s">
+      <c r="H8" s="48"/>
+      <c r="I8" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="J8" s="32"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="31" t="s">
+      <c r="J8" s="47"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="32"/>
-      <c r="N8" s="33"/>
-      <c r="O8" s="31" t="s">
+      <c r="M8" s="47"/>
+      <c r="N8" s="48"/>
+      <c r="O8" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="P8" s="32"/>
-      <c r="Q8" s="33"/>
-      <c r="R8" s="31" t="s">
+      <c r="P8" s="47"/>
+      <c r="Q8" s="48"/>
+      <c r="R8" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="S8" s="32"/>
-      <c r="T8" s="33"/>
-      <c r="U8" s="31" t="s">
+      <c r="S8" s="47"/>
+      <c r="T8" s="48"/>
+      <c r="U8" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="V8" s="32"/>
-      <c r="W8" s="33"/>
+      <c r="V8" s="47"/>
+      <c r="W8" s="48"/>
     </row>
     <row r="9" spans="1:23" ht="28.5">
       <c r="A9" s="6"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="7" t="s">
         <v>17</v>
       </c>
@@ -3021,7 +3028,7 @@
       <c r="C11" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D11" s="49" t="s">
+      <c r="D11" s="50" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="19" t="s">
@@ -3055,12 +3062,14 @@
       <c r="C12" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="49"/>
+      <c r="D12" s="50"/>
       <c r="E12" s="18" t="s">
         <v>87</v>
       </c>
       <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
+      <c r="G12" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="H12" s="11"/>
       <c r="I12" s="11" t="s">
         <v>111</v>
@@ -3087,12 +3096,14 @@
       <c r="C13" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="49"/>
+      <c r="D13" s="50"/>
       <c r="E13" s="18" t="s">
         <v>88</v>
       </c>
       <c r="F13" s="13"/>
-      <c r="G13" s="11"/>
+      <c r="G13" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="H13" s="11"/>
       <c r="I13" s="11" t="s">
         <v>111</v>
@@ -3117,7 +3128,7 @@
       <c r="C14" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="49"/>
+      <c r="D14" s="50"/>
       <c r="E14" s="18" t="s">
         <v>103</v>
       </c>
@@ -3147,7 +3158,7 @@
       <c r="C15" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D15" s="49"/>
+      <c r="D15" s="50"/>
       <c r="E15" s="27" t="s">
         <v>83</v>
       </c>
@@ -3179,12 +3190,14 @@
       <c r="C16" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="49"/>
+      <c r="D16" s="50"/>
       <c r="E16" s="18" t="s">
         <v>40</v>
       </c>
       <c r="F16" s="13"/>
-      <c r="G16" s="11"/>
+      <c r="G16" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="H16" s="11"/>
       <c r="I16" s="11" t="s">
         <v>111</v>
@@ -3211,7 +3224,7 @@
       <c r="C17" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D17" s="49"/>
+      <c r="D17" s="50"/>
       <c r="E17" s="18" t="s">
         <v>20</v>
       </c>
@@ -3243,7 +3256,7 @@
       <c r="C18" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D18" s="49"/>
+      <c r="D18" s="50"/>
       <c r="E18" s="18" t="s">
         <v>7</v>
       </c>
@@ -3275,7 +3288,7 @@
       <c r="C19" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D19" s="49"/>
+      <c r="D19" s="50"/>
       <c r="E19" s="18" t="s">
         <v>24</v>
       </c>
@@ -3287,7 +3300,9 @@
       <c r="I19" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="J19" s="11"/>
+      <c r="J19" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="K19" s="11" t="s">
         <v>122</v>
       </c>
@@ -3311,7 +3326,7 @@
       <c r="C20" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D20" s="49"/>
+      <c r="D20" s="50"/>
       <c r="E20" s="18" t="s">
         <v>64</v>
       </c>
@@ -3343,7 +3358,7 @@
       <c r="C21" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D21" s="49"/>
+      <c r="D21" s="50"/>
       <c r="E21" s="3" t="s">
         <v>65</v>
       </c>
@@ -3457,7 +3472,9 @@
       <c r="I24" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="J24" s="11"/>
+      <c r="J24" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="K24" s="11" t="s">
         <v>123</v>
       </c>
@@ -3495,7 +3512,9 @@
       <c r="I25" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="J25" s="11"/>
+      <c r="J25" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="K25" s="11"/>
       <c r="L25" s="11"/>
       <c r="M25" s="11"/>
@@ -4036,6 +4055,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:D3"/>
+    <mergeCell ref="E1:I3"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="C7:C9"/>
     <mergeCell ref="D11:D21"/>
     <mergeCell ref="L7:N7"/>
     <mergeCell ref="O7:Q7"/>
@@ -4047,15 +4075,6 @@
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="R8:T8"/>
     <mergeCell ref="U8:W8"/>
-    <mergeCell ref="B1:D3"/>
-    <mergeCell ref="E1:I3"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="C7:C9"/>
   </mergeCells>
   <conditionalFormatting sqref="G10:G41 I10:J41 L10:M41 O10:P41 R10:S41 U10:V41">
     <cfRule type="expression" dxfId="9" priority="4">
@@ -4087,11 +4106,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W45"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="C14" zoomScale="96" zoomScaleNormal="70" zoomScaleSheetLayoutView="96" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="F5" zoomScale="96" zoomScaleNormal="70" zoomScaleSheetLayoutView="96" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4118,16 +4137,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="37" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
       <c r="J1" s="2" t="s">
         <v>25</v>
       </c>
@@ -4136,28 +4155,28 @@
       </c>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
       <c r="J2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
       <c r="J3" s="2" t="s">
         <v>27</v>
       </c>
@@ -4197,94 +4216,94 @@
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:23">
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="43" t="s">
+      <c r="F7" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="34" t="s">
+      <c r="G7" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="34"/>
-      <c r="I7" s="28" t="s">
+      <c r="H7" s="49"/>
+      <c r="I7" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="29"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="28" t="s">
+      <c r="J7" s="44"/>
+      <c r="K7" s="45"/>
+      <c r="L7" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="29"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="28" t="s">
+      <c r="M7" s="44"/>
+      <c r="N7" s="45"/>
+      <c r="O7" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="28" t="s">
+      <c r="P7" s="44"/>
+      <c r="Q7" s="45"/>
+      <c r="R7" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="S7" s="29"/>
-      <c r="T7" s="30"/>
-      <c r="U7" s="28" t="s">
+      <c r="S7" s="44"/>
+      <c r="T7" s="45"/>
+      <c r="U7" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="V7" s="29"/>
-      <c r="W7" s="30"/>
+      <c r="V7" s="44"/>
+      <c r="W7" s="45"/>
     </row>
     <row r="8" spans="1:23">
-      <c r="B8" s="44"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="31" t="s">
+      <c r="B8" s="38"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="H8" s="33"/>
-      <c r="I8" s="31" t="s">
+      <c r="H8" s="48"/>
+      <c r="I8" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="J8" s="32"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="31" t="s">
+      <c r="J8" s="47"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="32"/>
-      <c r="N8" s="33"/>
-      <c r="O8" s="31" t="s">
+      <c r="M8" s="47"/>
+      <c r="N8" s="48"/>
+      <c r="O8" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="P8" s="32"/>
-      <c r="Q8" s="33"/>
-      <c r="R8" s="31" t="s">
+      <c r="P8" s="47"/>
+      <c r="Q8" s="48"/>
+      <c r="R8" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="S8" s="32"/>
-      <c r="T8" s="33"/>
-      <c r="U8" s="31" t="s">
+      <c r="S8" s="47"/>
+      <c r="T8" s="48"/>
+      <c r="U8" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="V8" s="32"/>
-      <c r="W8" s="33"/>
+      <c r="V8" s="47"/>
+      <c r="W8" s="48"/>
     </row>
     <row r="9" spans="1:23" ht="28.5">
       <c r="A9" s="6"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="7" t="s">
         <v>17</v>
       </c>
@@ -4344,7 +4363,7 @@
       <c r="C10" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D10" s="53" t="s">
+      <c r="D10" s="54" t="s">
         <v>34</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -4380,7 +4399,7 @@
       <c r="C11" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D11" s="54"/>
+      <c r="D11" s="55"/>
       <c r="E11" s="3" t="s">
         <v>47</v>
       </c>
@@ -4414,7 +4433,7 @@
       <c r="C12" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="54"/>
+      <c r="D12" s="55"/>
       <c r="E12" s="11" t="s">
         <v>56</v>
       </c>
@@ -4426,7 +4445,9 @@
       <c r="I12" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="J12" s="11"/>
+      <c r="J12" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="K12" s="11" t="s">
         <v>124</v>
       </c>
@@ -4450,7 +4471,7 @@
       <c r="C13" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="55"/>
+      <c r="D13" s="56"/>
       <c r="E13" s="11" t="s">
         <v>57</v>
       </c>
@@ -4520,7 +4541,7 @@
       <c r="C15" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D15" s="53" t="s">
+      <c r="D15" s="54" t="s">
         <v>43</v>
       </c>
       <c r="E15" s="11" t="s">
@@ -4556,7 +4577,7 @@
       <c r="C16" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="55"/>
+      <c r="D16" s="56"/>
       <c r="E16" s="11" t="s">
         <v>45</v>
       </c>
@@ -4588,7 +4609,7 @@
       <c r="C17" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D17" s="53" t="s">
+      <c r="D17" s="54" t="s">
         <v>46</v>
       </c>
       <c r="E17" s="13" t="s">
@@ -4624,7 +4645,7 @@
       <c r="C18" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D18" s="55"/>
+      <c r="D18" s="56"/>
       <c r="E18" s="13" t="s">
         <v>80</v>
       </c>
@@ -4658,7 +4679,7 @@
       <c r="C19" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D19" s="50" t="s">
+      <c r="D19" s="51" t="s">
         <v>48</v>
       </c>
       <c r="E19" s="13" t="s">
@@ -4672,8 +4693,10 @@
       <c r="I19" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="J19" s="11"/>
-      <c r="K19" s="59" t="s">
+      <c r="J19" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="K19" s="28" t="s">
         <v>125</v>
       </c>
       <c r="L19" s="11"/>
@@ -4694,7 +4717,7 @@
       <c r="C20" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D20" s="52"/>
+      <c r="D20" s="53"/>
       <c r="E20" s="26" t="s">
         <v>97</v>
       </c>
@@ -4704,7 +4727,9 @@
       <c r="I20" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="J20" s="11"/>
+      <c r="J20" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="K20" s="11"/>
       <c r="L20" s="11"/>
       <c r="M20" s="11"/>
@@ -4740,7 +4765,9 @@
       <c r="I21" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="J21" s="11"/>
+      <c r="J21" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="K21" s="11" t="s">
         <v>126</v>
       </c>
@@ -4764,7 +4791,7 @@
       <c r="C22" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D22" s="50" t="s">
+      <c r="D22" s="51" t="s">
         <v>50</v>
       </c>
       <c r="E22" s="13" t="s">
@@ -4800,7 +4827,7 @@
       <c r="C23" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D23" s="51"/>
+      <c r="D23" s="52"/>
       <c r="E23" s="3" t="s">
         <v>66</v>
       </c>
@@ -4832,7 +4859,7 @@
       <c r="C24" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D24" s="52"/>
+      <c r="D24" s="53"/>
       <c r="E24" s="11" t="s">
         <v>68</v>
       </c>
@@ -4866,7 +4893,7 @@
       <c r="C25" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D25" s="53" t="s">
+      <c r="D25" s="54" t="s">
         <v>52</v>
       </c>
       <c r="E25" s="11" t="s">
@@ -4902,7 +4929,7 @@
       <c r="C26" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D26" s="54"/>
+      <c r="D26" s="55"/>
       <c r="E26" s="13" t="s">
         <v>59</v>
       </c>
@@ -4934,7 +4961,7 @@
       <c r="C27" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D27" s="54"/>
+      <c r="D27" s="55"/>
       <c r="E27" s="13" t="s">
         <v>69</v>
       </c>
@@ -4968,7 +4995,7 @@
       <c r="C28" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D28" s="54"/>
+      <c r="D28" s="55"/>
       <c r="E28" s="13" t="s">
         <v>60</v>
       </c>
@@ -5002,7 +5029,7 @@
       <c r="C29" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D29" s="54"/>
+      <c r="D29" s="55"/>
       <c r="E29" s="15" t="s">
         <v>62</v>
       </c>
@@ -5034,7 +5061,7 @@
       <c r="C30" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D30" s="54"/>
+      <c r="D30" s="55"/>
       <c r="E30" s="14" t="s">
         <v>74</v>
       </c>
@@ -5066,7 +5093,7 @@
       <c r="C31" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D31" s="55"/>
+      <c r="D31" s="56"/>
       <c r="E31" s="23" t="s">
         <v>81</v>
       </c>
@@ -5463,6 +5490,21 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="D25:D31"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="B1:D3"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E1:I3"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="C7:C9"/>
     <mergeCell ref="U7:W7"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="I8:K8"/>
@@ -5473,21 +5515,6 @@
     <mergeCell ref="L7:N7"/>
     <mergeCell ref="O7:Q7"/>
     <mergeCell ref="R7:T7"/>
-    <mergeCell ref="E1:I3"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="D25:D31"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="B1:D3"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D19:D20"/>
   </mergeCells>
   <conditionalFormatting sqref="G10:G43 L10:M43 O10:P43 R10:S43 U10:V43 I10:J43">
     <cfRule type="expression" dxfId="6" priority="4">
@@ -5519,7 +5546,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V44"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="C8" zoomScale="96" zoomScaleSheetLayoutView="96" workbookViewId="0">
@@ -5549,15 +5576,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="37" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
       <c r="I1" s="2" t="s">
         <v>25</v>
       </c>
@@ -5566,26 +5593,26 @@
       </c>
     </row>
     <row r="2" spans="1:22" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
       <c r="I2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:22" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
       <c r="I3" s="2" t="s">
         <v>27</v>
       </c>
@@ -5622,89 +5649,89 @@
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:22">
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="34" t="s">
+      <c r="F7" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="34"/>
-      <c r="H7" s="28" t="s">
+      <c r="G7" s="49"/>
+      <c r="H7" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="29"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="28" t="s">
+      <c r="I7" s="44"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="29"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="28" t="s">
+      <c r="L7" s="44"/>
+      <c r="M7" s="45"/>
+      <c r="N7" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="29"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="28" t="s">
+      <c r="O7" s="44"/>
+      <c r="P7" s="45"/>
+      <c r="Q7" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="R7" s="29"/>
-      <c r="S7" s="30"/>
-      <c r="T7" s="28" t="s">
+      <c r="R7" s="44"/>
+      <c r="S7" s="45"/>
+      <c r="T7" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="U7" s="29"/>
-      <c r="V7" s="30"/>
+      <c r="U7" s="44"/>
+      <c r="V7" s="45"/>
     </row>
     <row r="8" spans="1:22">
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="31" t="s">
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="33"/>
-      <c r="H8" s="31" t="s">
+      <c r="G8" s="48"/>
+      <c r="H8" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="32"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="31" t="s">
+      <c r="I8" s="47"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="L8" s="32"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="31" t="s">
+      <c r="L8" s="47"/>
+      <c r="M8" s="48"/>
+      <c r="N8" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="O8" s="32"/>
-      <c r="P8" s="33"/>
-      <c r="Q8" s="31" t="s">
+      <c r="O8" s="47"/>
+      <c r="P8" s="48"/>
+      <c r="Q8" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="R8" s="32"/>
-      <c r="S8" s="33"/>
-      <c r="T8" s="31" t="s">
+      <c r="R8" s="47"/>
+      <c r="S8" s="48"/>
+      <c r="T8" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="U8" s="32"/>
-      <c r="V8" s="33"/>
+      <c r="U8" s="47"/>
+      <c r="V8" s="48"/>
     </row>
     <row r="9" spans="1:22" ht="28.5">
       <c r="A9" s="6"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
       <c r="F9" s="7" t="s">
         <v>17</v>
       </c>
@@ -5761,7 +5788,7 @@
       <c r="B10" s="9">
         <v>1</v>
       </c>
-      <c r="C10" s="56" t="s">
+      <c r="C10" s="57" t="s">
         <v>34</v>
       </c>
       <c r="D10" s="11" t="s">
@@ -5790,7 +5817,7 @@
       <c r="B11" s="9">
         <v>2</v>
       </c>
-      <c r="C11" s="57"/>
+      <c r="C11" s="58"/>
       <c r="D11" s="11" t="s">
         <v>67</v>
       </c>
@@ -5817,7 +5844,7 @@
       <c r="B12" s="9">
         <v>3</v>
       </c>
-      <c r="C12" s="57"/>
+      <c r="C12" s="58"/>
       <c r="D12" s="13" t="s">
         <v>77</v>
       </c>
@@ -5844,7 +5871,7 @@
       <c r="B13" s="9">
         <v>4</v>
       </c>
-      <c r="C13" s="57"/>
+      <c r="C13" s="58"/>
       <c r="D13" s="13" t="s">
         <v>78</v>
       </c>
@@ -5871,7 +5898,7 @@
       <c r="B14" s="9">
         <v>5</v>
       </c>
-      <c r="C14" s="57"/>
+      <c r="C14" s="58"/>
       <c r="D14" s="11" t="s">
         <v>94</v>
       </c>
@@ -5898,7 +5925,7 @@
       <c r="B15" s="9">
         <v>6</v>
       </c>
-      <c r="C15" s="57"/>
+      <c r="C15" s="58"/>
       <c r="D15" s="13" t="s">
         <v>95</v>
       </c>
@@ -5925,7 +5952,7 @@
       <c r="B16" s="9">
         <v>7</v>
       </c>
-      <c r="C16" s="58"/>
+      <c r="C16" s="59"/>
       <c r="D16" s="13" t="s">
         <v>96</v>
       </c>
@@ -6647,6 +6674,15 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C10:C16"/>
+    <mergeCell ref="B1:C3"/>
+    <mergeCell ref="D1:H3"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:J7"/>
     <mergeCell ref="K7:M7"/>
     <mergeCell ref="N7:P7"/>
     <mergeCell ref="Q7:S7"/>
@@ -6657,15 +6693,6 @@
     <mergeCell ref="N8:P8"/>
     <mergeCell ref="Q8:S8"/>
     <mergeCell ref="T8:V8"/>
-    <mergeCell ref="C10:C16"/>
-    <mergeCell ref="B1:C3"/>
-    <mergeCell ref="D1:H3"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:J7"/>
   </mergeCells>
   <conditionalFormatting sqref="F10:F40 H10:I40 K10:L40 N10:O40 Q10:R40 T10:U40">
     <cfRule type="expression" dxfId="3" priority="4">

</xml_diff>

<commit_message>
chỉnh sửa dữ liệu sau khi review
</commit_message>
<xml_diff>
--- a/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Cap nhat dia diem/CF0142_BAChecklistERP.xlsx
+++ b/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Cap nhat dia diem/CF0142_BAChecklistERP.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SOFT\201512\10_DOCUMENT\13_DETAIL_DESIGN\Cap nhat dia diem\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" tabRatio="653"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" tabRatio="653" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Layout" sheetId="1" r:id="rId1"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="127">
   <si>
     <t>STT</t>
   </si>
@@ -417,7 +422,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -739,9 +744,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -784,6 +786,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -819,42 +824,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -1155,7 +1125,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1187,9 +1157,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1221,6 +1192,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1396,11 +1368,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y44"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="93" zoomScaleSheetLayoutView="93" workbookViewId="0">
-      <pane xSplit="5" ySplit="9" topLeftCell="I10" activePane="bottomRight" state="frozen"/>
+    <sheetView view="pageBreakPreview" zoomScale="93" zoomScaleSheetLayoutView="93" workbookViewId="0">
+      <pane xSplit="5" ySplit="9" topLeftCell="F10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
       <selection pane="bottomRight" activeCell="W15" sqref="W15"/>
@@ -1432,16 +1404,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="39" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
       <c r="J1" s="2" t="s">
         <v>25</v>
       </c>
@@ -1450,28 +1422,28 @@
       </c>
     </row>
     <row r="2" spans="1:25" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
       <c r="J2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:25" s="1" customFormat="1" ht="15.75">
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
       <c r="J3" s="2" t="s">
         <v>27</v>
       </c>
@@ -1513,25 +1485,25 @@
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:25">
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="E7" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="45" t="s">
+      <c r="F7" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="36" t="s">
+      <c r="G7" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="36"/>
+      <c r="H7" s="50"/>
       <c r="I7" s="30" t="s">
         <v>8</v>
       </c>
@@ -1561,11 +1533,11 @@
       <c r="Y7" s="32"/>
     </row>
     <row r="8" spans="1:25">
-      <c r="B8" s="46"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
       <c r="G8" s="33" t="s">
         <v>113</v>
       </c>
@@ -1600,11 +1572,11 @@
     </row>
     <row r="9" spans="1:25" ht="28.5">
       <c r="A9" s="6"/>
-      <c r="B9" s="47"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
       <c r="G9" s="7" t="s">
         <v>17</v>
       </c>
@@ -1670,7 +1642,7 @@
       <c r="C10" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="36" t="s">
         <v>34</v>
       </c>
       <c r="E10" s="18" t="s">
@@ -1708,7 +1680,7 @@
       <c r="C11" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D11" s="37"/>
+      <c r="D11" s="36"/>
       <c r="E11" s="19" t="s">
         <v>36</v>
       </c>
@@ -1744,7 +1716,7 @@
       <c r="C12" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="37"/>
+      <c r="D12" s="36"/>
       <c r="E12" s="19" t="s">
         <v>37</v>
       </c>
@@ -1780,7 +1752,7 @@
       <c r="C13" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="37"/>
+      <c r="D13" s="36"/>
       <c r="E13" s="18" t="s">
         <v>39</v>
       </c>
@@ -1816,7 +1788,7 @@
       <c r="C14" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D14" s="37"/>
+      <c r="D14" s="36"/>
       <c r="E14" s="18" t="s">
         <v>35</v>
       </c>
@@ -1850,7 +1822,7 @@
       <c r="C15" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D15" s="37"/>
+      <c r="D15" s="36"/>
       <c r="E15" s="20" t="s">
         <v>63</v>
       </c>
@@ -2763,6 +2735,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="L8:M8"/>
     <mergeCell ref="W7:Y7"/>
     <mergeCell ref="W8:Y8"/>
     <mergeCell ref="D10:D15"/>
@@ -2779,15 +2757,9 @@
     <mergeCell ref="Q7:S7"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="I7:K7"/>
-    <mergeCell ref="N8:P8"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="L8:M8"/>
   </mergeCells>
   <conditionalFormatting sqref="G10:G43 I10:J43 L10:L43 N10:O43 Q10:R43 T10:U43 W10:X43">
-    <cfRule type="expression" dxfId="8" priority="16">
+    <cfRule type="expression" dxfId="6" priority="16">
       <formula>G10="NG"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2803,11 +2775,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z43"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="E10" zoomScale="85" zoomScaleNormal="55" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A19" zoomScale="85" zoomScaleNormal="55" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="X24" sqref="X24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2836,16 +2808,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="39" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
       <c r="J1" s="2" t="s">
         <v>25</v>
       </c>
@@ -2854,28 +2826,28 @@
       </c>
     </row>
     <row r="2" spans="1:26" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
       <c r="J2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:26" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
       <c r="J3" s="2" t="s">
         <v>27</v>
       </c>
@@ -2915,25 +2887,25 @@
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:26">
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="E7" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="45" t="s">
+      <c r="F7" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="36" t="s">
+      <c r="G7" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="36"/>
+      <c r="H7" s="50"/>
       <c r="I7" s="30" t="s">
         <v>8</v>
       </c>
@@ -2966,11 +2938,11 @@
       <c r="Z7" s="32"/>
     </row>
     <row r="8" spans="1:26">
-      <c r="B8" s="46"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
       <c r="G8" s="33" t="s">
         <v>114</v>
       </c>
@@ -3008,11 +2980,11 @@
     </row>
     <row r="9" spans="1:26" ht="28.5">
       <c r="A9" s="6"/>
-      <c r="B9" s="47"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
       <c r="G9" s="7" t="s">
         <v>17</v>
       </c>
@@ -3437,7 +3409,9 @@
       <c r="X19" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="Y19" s="11"/>
+      <c r="Y19" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="Z19" s="11"/>
     </row>
     <row r="20" spans="2:26">
@@ -4252,6 +4226,15 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B1:D3"/>
+    <mergeCell ref="E1:I3"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="C7:C9"/>
     <mergeCell ref="X7:Z7"/>
     <mergeCell ref="X8:Z8"/>
     <mergeCell ref="D11:D21"/>
@@ -4265,18 +4248,9 @@
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="R8:T8"/>
     <mergeCell ref="U8:W8"/>
-    <mergeCell ref="B1:D3"/>
-    <mergeCell ref="E1:I3"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="C7:C9"/>
   </mergeCells>
   <conditionalFormatting sqref="G10:G43 I10:J43 L10:M43 O10:P43 R10:S43 U10:V43 X10:Y43">
-    <cfRule type="expression" dxfId="4" priority="7">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>G10="NG"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4292,11 +4266,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z45"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="E1" zoomScale="85" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScale="85" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="Y21" sqref="Y21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4325,16 +4299,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="39" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
       <c r="J1" s="2" t="s">
         <v>25</v>
       </c>
@@ -4343,28 +4317,28 @@
       </c>
     </row>
     <row r="2" spans="1:26" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
       <c r="J2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:26" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
       <c r="J3" s="2" t="s">
         <v>27</v>
       </c>
@@ -4404,25 +4378,25 @@
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:26">
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="E7" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="45" t="s">
+      <c r="F7" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="36" t="s">
+      <c r="G7" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="36"/>
+      <c r="H7" s="50"/>
       <c r="I7" s="30" t="s">
         <v>8</v>
       </c>
@@ -4455,11 +4429,11 @@
       <c r="Z7" s="32"/>
     </row>
     <row r="8" spans="1:26">
-      <c r="B8" s="46"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
       <c r="G8" s="33" t="s">
         <v>113</v>
       </c>
@@ -4497,11 +4471,11 @@
     </row>
     <row r="9" spans="1:26" ht="28.5">
       <c r="A9" s="6"/>
-      <c r="B9" s="47"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
       <c r="G9" s="7" t="s">
         <v>17</v>
       </c>
@@ -5032,7 +5006,9 @@
       <c r="X21" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="Y21" s="11"/>
+      <c r="Y21" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="Z21" s="11"/>
     </row>
     <row r="22" spans="2:26">
@@ -5813,6 +5789,21 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="D25:D31"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="B1:D3"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E1:I3"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="C7:C9"/>
     <mergeCell ref="X7:Z7"/>
     <mergeCell ref="X8:Z8"/>
     <mergeCell ref="U7:W7"/>
@@ -5825,24 +5816,9 @@
     <mergeCell ref="L7:N7"/>
     <mergeCell ref="O7:Q7"/>
     <mergeCell ref="R7:T7"/>
-    <mergeCell ref="E1:I3"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="D25:D31"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="B1:D3"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D19:D20"/>
   </mergeCells>
   <conditionalFormatting sqref="G10:G45 I10:J45 L10:M45 O10:P45 R10:S45 U10:V45 X10:Y45">
-    <cfRule type="expression" dxfId="0" priority="7">
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>G10="NG"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5858,7 +5834,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V44"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="C8" zoomScale="96" zoomScaleSheetLayoutView="96" workbookViewId="0">
@@ -5888,15 +5864,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="39" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
       <c r="I1" s="2" t="s">
         <v>25</v>
       </c>
@@ -5905,26 +5881,26 @@
       </c>
     </row>
     <row r="2" spans="1:22" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
       <c r="I2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:22" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
       <c r="I3" s="2" t="s">
         <v>27</v>
       </c>
@@ -5961,22 +5937,22 @@
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:22">
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="E7" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="36" t="s">
+      <c r="F7" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="36"/>
+      <c r="G7" s="50"/>
       <c r="H7" s="30" t="s">
         <v>8</v>
       </c>
@@ -6004,10 +5980,10 @@
       <c r="V7" s="32"/>
     </row>
     <row r="8" spans="1:22">
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
       <c r="F8" s="33" t="s">
         <v>16</v>
       </c>
@@ -6040,10 +6016,10 @@
     </row>
     <row r="9" spans="1:22" ht="28.5">
       <c r="A9" s="6"/>
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
       <c r="F9" s="7" t="s">
         <v>17</v>
       </c>
@@ -6986,6 +6962,15 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C10:C16"/>
+    <mergeCell ref="B1:C3"/>
+    <mergeCell ref="D1:H3"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:J7"/>
     <mergeCell ref="K7:M7"/>
     <mergeCell ref="N7:P7"/>
     <mergeCell ref="Q7:S7"/>
@@ -6996,33 +6981,24 @@
     <mergeCell ref="N8:P8"/>
     <mergeCell ref="Q8:S8"/>
     <mergeCell ref="T8:V8"/>
-    <mergeCell ref="C10:C16"/>
-    <mergeCell ref="B1:C3"/>
-    <mergeCell ref="D1:H3"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:J7"/>
   </mergeCells>
   <conditionalFormatting sqref="F10:F40 H10:I40 K10:L40 N10:O40 Q10:R40 T10:U40">
-    <cfRule type="expression" dxfId="13" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>F10="NG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F41 H41:I41 K41:L41 N41:O41 Q41:R41 T41:U41">
-    <cfRule type="expression" dxfId="12" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>F41="NG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F42 H42:I42 K42:L42 N42:O42 Q42:R42 T42:U42">
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>F42="NG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F43 H43:I43 K43:L43 N43:O43 Q43:R43 T43:U43">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>F43="NG"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>